<commit_message>
V0.2.33.1: Arrumado bug da Quest dos Yets
V0.2.33.1: Arrumado bug da Quest dos Yets

_____________________________________________

Como estou na fase de revisão (ainda terei á de padronização), você vai perceber que a cada atualização, as falas/textos e o jogo parece estar mais fluido, e as conversas estão mais naturais. (Os nomes das Cidades ainda não são permanentes, pois percebi que em algumas partes do jogo, elas não podem ser traduzidas, então provavelmente terei de coloca-las em inglês, após terminar as reviões)
</commit_message>
<xml_diff>
--- a/default-files/Example_ExcelReference/excel/沙盒/Localization/english/R任务列表_Quests_19k_hotfix.xlsx
+++ b/default-files/Example_ExcelReference/excel/沙盒/Localization/english/R任务列表_Quests_19k_hotfix.xlsx
@@ -1,32 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Users\isyuricunha\Documents\GitHub\sands-of-salzaar-game-translation\default-files\Example_ExcelReference\excel\沙盒\Localization\english\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D88A276-716B-4F7F-B381-47637A85D044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540"/>
+    <workbookView xWindow="90" yWindow="630" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="main" sheetId="3" r:id="rId5"/>
+    <sheet name="main" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525" fullCalcOnLoad="1"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <d:author xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">Administrator</d:author>
+    <author>Administrator</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
-        <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+        <r>
           <rPr>
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">任务子项格式说明:
+          <t>任务子项格式说明:
 子项1类型#描述文字#数目#绑定目标#追踪位置
 子项2类型#描述文字#数目#绑定目标#追踪位置
 ...
@@ -47,7 +53,7 @@
 只有当子项未满足时才会进行地图标记显示
 子项参数的数目可以填0，当为0时默认子项已经完成
 当所有子项已经完成时，默认任务是完成状态</t>
-        </d:r>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -55,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="251">
   <si>
     <t>任务ID_QuestID</t>
   </si>
@@ -222,11 +228,11 @@
     <t>Amar is looking for a Patterned Shell and a Tripoint Shell. The town of Agadir in Twinluna Valley should have some for sale.</t>
   </si>
   <si>
-    <t xml:space="preserve">4#收集花纹贝壳×1并交给阿默尔#1#花纹贝壳#沙盒双月山谷:-2017,-268:100|PLACE:浅溪镇
+    <t>4#收集花纹贝壳×1并交给阿默尔#1#花纹贝壳#沙盒双月山谷:-2017,-268:100|PLACE:浅溪镇
 4#收集三褶贝壳×1并交给阿默尔#1#三褶贝壳#沙盒双月山谷:-2017,-268:100|PLACE:浅溪镇</t>
   </si>
   <si>
-    <t xml:space="preserve">4#Retrieve a Patterned Shell for Amar#1#花纹贝壳#沙盒双月山谷:-2017,-268:100|PLACE:浅溪镇
+    <t>4#Retrieve a Patterned Shell for Amar#1#花纹贝壳#沙盒双月山谷:-2017,-268:100|PLACE:浅溪镇
 4#Retrieve a Tripoint Shell for Amar#1#三褶贝壳#沙盒双月山谷:-2017,-268:100|PLACE:浅溪镇</t>
   </si>
   <si>
@@ -242,12 +248,12 @@
     <t>Rajif is cooking up the perfect banquet and is looking for one piece each of Exquisite Beef, Exquisite Lamb and Exquisite Chicken.</t>
   </si>
   <si>
-    <t xml:space="preserve">4#收集精致牛肉×1并交给热伊#1#精致牛肉#
+    <t>4#收集精致牛肉×1并交给热伊#1#精致牛肉#
 4#收集精致鸡肉×1并交给热伊#1#精致鸡肉#
 4#收集精致羊肉×1并交给热伊#1#精致羊肉#</t>
   </si>
   <si>
-    <t xml:space="preserve">4#Retrieve Exquisite Beef for Rajif#1#精致牛肉#
+    <t>4#Retrieve Exquisite Beef for Rajif#1#精致牛肉#
 4#Retrieve Exquisite Chicken for Rajif#1#精致鸡肉#
 4#Retrieve Exquisite Lamb for Rajif#1#精致羊肉#</t>
   </si>
@@ -264,13 +270,13 @@
     <t>Dariush is cooking up the perfect banquet and is looking for one piece each of a Golden Mushroom, Penny Bun, Stinkhorn, and Tashashu Mushroom.</t>
   </si>
   <si>
-    <t xml:space="preserve">4#收集金针菇×3并交给青岩#3#金针菇#
+    <t>4#收集金针菇×3并交给青岩#3#金针菇#
 4#收集牛肝菌×3并交给青岩#3#牛肝菌#
 4#收集金针菇×3并交给青岩#3#茶树菇#
 4#收集金针菇×3并交给青岩#3#竹荪#</t>
   </si>
   <si>
-    <t xml:space="preserve">4#Retrieve 3 Golden Mushrooms for Dariush#3#金针菇#
+    <t>4#Retrieve 3 Golden Mushrooms for Dariush#3#金针菇#
 4#Retrieve 3 Penny Buns for Darius#3#牛肝菌#
 4#Retrieve 3 Tashashu Mushroom for Dariush#3#茶树菇#
 4#Retrieve 3 Stinkhorns for Dariush#3#竹荪#</t>
@@ -378,11 +384,11 @@
     <t>Amir hopes you can fight off 3 squads of Ifrit Laborers.</t>
   </si>
   <si>
-    <t xml:space="preserve">3#驱逐10个火魔苦工#10#火魔苦工#
+    <t>3#驱逐10个火魔苦工#10#火魔苦工#
 3#驱逐10个火魔奴隶#10#火魔奴隶#</t>
   </si>
   <si>
-    <t xml:space="preserve">3#Defeat 10 Ifrit Laborers#10#火魔苦工#
+    <t>3#Defeat 10 Ifrit Laborers#10#火魔苦工#
 3#Defeat 10 Ifrit Slaves#10#火魔奴隶#</t>
   </si>
   <si>
@@ -512,15 +518,9 @@
     <t>淼淼拜托你去不远处的山洞找回她丢失的物品，要小心隐藏地底的雪怪</t>
   </si>
   <si>
-    <t>Marwa pleads for you to visit a nearby cave and help retrieve her lost items. Be careful though - Yeti lurk within.</t>
-  </si>
-  <si>
     <t>0#击败雪怪#1##大雪山:1971,1332:0|CHEST:灰雪雪怪山洞</t>
   </si>
   <si>
-    <t>0#Defeat the Yeti#1##大雪山:1971,1332:0|CHEST:灰雪雪怪山洞</t>
-  </si>
-  <si>
     <t>青石村</t>
   </si>
   <si>
@@ -551,12 +551,12 @@
     <t>Collect three samples of Honeysuckle in the woods to the north and west of the town.</t>
   </si>
   <si>
-    <t xml:space="preserve">0#采集忍冬草A#1|CHEST:青石村找回药草1
+    <t>0#采集忍冬草A#1|CHEST:青石村找回药草1
 0#采集忍冬草B#1|CHEST:青石村找回药草2
 0#采集忍冬草C#1|CHEST:青石村找回药草3</t>
   </si>
   <si>
-    <t xml:space="preserve">0#Collect Honeysuckle A#1|CHEST:青石村找回药草1
+    <t>0#Collect Honeysuckle A#1|CHEST:青石村找回药草1
 0#Collect Honeysuckle B#1|CHEST:青石村找回药草2
 0#Collect Honeysuckle C#1|CHEST:青石村找回药草3</t>
   </si>
@@ -735,7 +735,7 @@
     <t>老乞丐告诉你沙漠废墟里的一个秘密和三个字——无尽城</t>
   </si>
   <si>
-    <t xml:space="preserve">The beggar tells you about a secret lying in the desert ruins. He whispers but two words:  E n d l e s s  C i t y.</t>
+    <t>The beggar tells you about a secret lying in the desert ruins. He whispers but two words:  E n d l e s s  C i t y.</t>
   </si>
   <si>
     <t>0#前往调查沙漠深处的废墟#1##大沙漠:638,7259:250</t>
@@ -826,19 +826,19 @@
   </si>
   <si>
     <t>0#Explore the Endless City#1##大沙漠:285,7337:0</t>
+  </si>
+  <si>
+    <t>Marwa implora para que você visite uma caverna próxima e a ajude a recuperar seus itens perdidos. Tenha cuidado - existem la dentro Yetis.</t>
+  </si>
+  <si>
+    <t>0#Derrote o Yeti.#1##大雪山:1971,1332:0|CHEST:灰雪雪怪山洞</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -851,131 +851,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
     </font>
@@ -985,8 +860,17 @@
       <color rgb="FF000000"/>
       <name val="宋体"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="39">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -995,187 +879,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="29"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1199,11 +903,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEA04" tint="0"/>
+        <fgColor rgb="FFFFEA04"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1228,518 +932,85 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="2">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="2">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="4">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="62">
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" applyNumberFormat="1" fontId="4" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="2" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="11" applyFill="1" borderId="2" applyBorder="1" xfId="3" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" applyNumberFormat="1" fontId="4" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="4" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" applyNumberFormat="1" fontId="4" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="5" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="14" applyFill="1" borderId="0" applyBorder="1" xfId="6" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="7" applyFill="1" borderId="0" applyBorder="1" xfId="7" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" applyNumberFormat="1" fontId="4" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="8" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="17" applyFill="1" borderId="0" applyBorder="1" xfId="9" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="10" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="10" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="11" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" applyNumberFormat="1" fontId="4" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="12" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="5" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="13" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="14" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="12" applyFill="1" borderId="3" applyBorder="1" xfId="15" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="22" applyFill="1" borderId="0" applyBorder="1" xfId="16" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="17" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="13" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="18" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="16" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="19" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="9" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="20" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="21" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="17" applyFont="1" fillId="0" applyFill="1" borderId="6" applyBorder="1" xfId="22" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="12" applyFont="1" fillId="0" applyFill="1" borderId="6" applyBorder="1" xfId="23" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="23" applyFill="1" borderId="0" applyBorder="1" xfId="24" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" borderId="5" applyBorder="1" xfId="25" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="20" applyFill="1" borderId="0" applyBorder="1" xfId="26" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="15" applyFont="1" fillId="24" applyFill="1" borderId="7" applyBorder="1" xfId="27" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="14" applyFont="1" fillId="24" applyFill="1" borderId="2" applyBorder="1" xfId="28" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="8" applyFont="1" fillId="16" applyFill="1" borderId="4" applyBorder="1" xfId="29" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="30" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="10" applyFill="1" borderId="0" applyBorder="1" xfId="31" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="18" applyFont="1" fillId="0" applyFill="1" borderId="8" applyBorder="1" xfId="32" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="20" applyFont="1" fillId="0" applyFill="1" borderId="9" applyBorder="1" xfId="33" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="19" applyFont="1" fillId="26" applyFill="1" borderId="0" applyBorder="1" xfId="34" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="11" applyFont="1" fillId="21" applyFill="1" borderId="0" applyBorder="1" xfId="35" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="29" applyFill="1" borderId="0" applyBorder="1" xfId="36" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="25" applyFill="1" borderId="0" applyBorder="1" xfId="37" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="5" applyFill="1" borderId="0" applyBorder="1" xfId="38" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="9" applyFill="1" borderId="0" applyBorder="1" xfId="39" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="6" applyFill="1" borderId="0" applyBorder="1" xfId="40" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="15" applyFill="1" borderId="0" applyBorder="1" xfId="41" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="28" applyFill="1" borderId="0" applyBorder="1" xfId="42" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="13" applyFill="1" borderId="0" applyBorder="1" xfId="43" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="44" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="19" applyFill="1" borderId="0" applyBorder="1" xfId="45" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="32" applyFill="1" borderId="0" applyBorder="1" xfId="46" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="31" applyFill="1" borderId="0" applyBorder="1" xfId="47" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="30" applyFill="1" borderId="0" applyBorder="1" xfId="48" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="18" applyFill="1" borderId="0" applyBorder="1" xfId="49" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="27" applyFill="1" borderId="0" applyBorder="1" xfId="50" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="8" applyFill="1" borderId="0" applyBorder="1" xfId="51" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="52" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="21" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="14" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="21" applyFont="1" fillId="34" applyFill="1" borderId="1" applyBorder="1" xfId="7" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="21" applyFont="1" fillId="35" applyFill="1" borderId="1" applyBorder="1" xfId="7" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="21" applyFont="1" fillId="36" applyFill="1" borderId="1" applyBorder="1" xfId="7" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="21" applyFont="1" fillId="33" applyFill="1" borderId="1" applyBorder="1" xfId="7" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="22" applyFont="1" fillId="37" applyFill="1" borderId="1" applyBorder="1" xfId="7" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="38" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="53">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="普通" xfId="11"/>
-    <cellStyle name="百分比" xfId="12" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="13" builtinId="9"/>
-    <cellStyle name="普通 2" xfId="14"/>
-    <cellStyle name="注释" xfId="15" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="16" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="17" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="18" builtinId="11"/>
-    <cellStyle name="标题" xfId="19" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="20" builtinId="53"/>
-    <cellStyle name="普通 4" xfId="21"/>
-    <cellStyle name="标题 1" xfId="22" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="23" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="24" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="25" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="26" builtinId="44"/>
-    <cellStyle name="输出" xfId="27" builtinId="21"/>
-    <cellStyle name="计算" xfId="28" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="29" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="30" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="31" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="32" builtinId="24"/>
-    <cellStyle name="汇总" xfId="33" builtinId="25"/>
-    <cellStyle name="好" xfId="34" builtinId="26"/>
-    <cellStyle name="适中" xfId="35" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="36" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="37" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="38" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="39" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="40" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="41" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="42" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="43" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="44" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="45" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="46" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="47" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="48" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="49" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="50" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="51" builtinId="52"/>
-    <cellStyle name="普通 3" xfId="52"/>
+  <cellStyles count="6">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="普通" xfId="2" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="普通 2" xfId="3" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="普通 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="普通 4" xfId="4" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2068,1028 +1339,1037 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I24" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="3" max="3" width="33.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="147" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="195.125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:9" ht="67.5">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="60" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="59" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="59" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="60" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="55" t="s">
+    <row r="2" spans="1:9" ht="81">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="55"/>
-      <c r="F2" s="55" t="s">
+      <c r="D2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="61" t="s">
+      <c r="G2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="61" t="s">
+      <c r="I2" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="55" t="s">
+    <row r="3" spans="1:9" ht="94.5">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="55"/>
-      <c r="F3" s="55" t="s">
+      <c r="D3" s="2"/>
+      <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="61" t="s">
+      <c r="G3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="55" t="s">
+      <c r="H3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="61" t="s">
+      <c r="I3" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="55" t="s">
+    <row r="4" spans="1:9" ht="108">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="F4" s="55" t="s">
+      <c r="D4" s="2"/>
+      <c r="F4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="61" t="s">
+      <c r="G4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="55" t="s">
+      <c r="H4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="61" t="s">
+      <c r="I4" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="55" t="s">
+    <row r="5" spans="1:9" ht="108">
+      <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="61" t="s">
+      <c r="C5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="55"/>
-      <c r="F5" s="55" t="s">
+      <c r="D5" s="2"/>
+      <c r="F5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="61" t="s">
+      <c r="G5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="55" t="s">
+      <c r="H5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="61" t="s">
+      <c r="I5" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="56" t="s">
+    <row r="6" spans="1:9" ht="67.5">
+      <c r="A6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="61" t="s">
+      <c r="C6" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="56"/>
-      <c r="F6" s="56" t="s">
+      <c r="D6" s="3"/>
+      <c r="F6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="61" t="s">
+      <c r="G6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="56" t="s">
+      <c r="H6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="61" t="s">
+      <c r="I6" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="56" t="s">
+    <row r="7" spans="1:9" ht="67.5">
+      <c r="A7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="56"/>
-      <c r="F7" s="56" t="s">
+      <c r="D7" s="3"/>
+      <c r="F7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="61" t="s">
+      <c r="G7" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="56" t="s">
+      <c r="H7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="61" t="s">
+      <c r="I7" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="57" t="s">
+    <row r="8" spans="1:9" ht="108">
+      <c r="A8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="61" t="s">
+      <c r="C8" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="57"/>
-      <c r="F8" s="57" t="s">
+      <c r="D8" s="4"/>
+      <c r="F8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="61" t="s">
+      <c r="G8" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="57" t="s">
+      <c r="H8" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="61" t="s">
+      <c r="I8" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="55" t="s">
+    <row r="9" spans="1:9" ht="297">
+      <c r="A9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="61" t="s">
+      <c r="C9" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="55"/>
-      <c r="F9" s="55" t="s">
+      <c r="D9" s="2"/>
+      <c r="F9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="61" t="s">
+      <c r="G9" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="55" t="s">
+      <c r="H9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="61" t="s">
+      <c r="I9" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="56" t="s">
+    <row r="10" spans="1:9" ht="243">
+      <c r="A10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="61" t="s">
+      <c r="C10" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="56"/>
-      <c r="F10" s="56" t="s">
+      <c r="D10" s="3"/>
+      <c r="F10" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G10" s="61" t="s">
+      <c r="G10" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H10" s="56" t="s">
+      <c r="H10" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I10" s="61" t="s">
+      <c r="I10" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="56" t="s">
+    <row r="11" spans="1:9" ht="270">
+      <c r="A11" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="61" t="s">
+      <c r="C11" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="56"/>
-      <c r="F11" s="56" t="s">
+      <c r="D11" s="3"/>
+      <c r="F11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="61" t="s">
+      <c r="G11" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="H11" s="56" t="s">
+      <c r="H11" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="I11" s="61" t="s">
+      <c r="I11" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="57" t="s">
+    <row r="12" spans="1:9" ht="40.5">
+      <c r="A12" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="57" t="s">
+      <c r="B12" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="61" t="s">
+      <c r="C12" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="57"/>
-      <c r="F12" s="57" t="s">
+      <c r="D12" s="4"/>
+      <c r="F12" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="G12" s="61" t="s">
+      <c r="G12" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="H12" s="57" t="s">
+      <c r="H12" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="I12" s="61" t="s">
+      <c r="I12" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="57" t="s">
+    <row r="13" spans="1:9" ht="54">
+      <c r="A13" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="61" t="s">
+      <c r="C13" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="57"/>
-      <c r="F13" s="57" t="s">
+      <c r="D13" s="4"/>
+      <c r="F13" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G13" s="61" t="s">
+      <c r="G13" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="H13" s="57" t="s">
+      <c r="H13" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="I13" s="61" t="s">
+      <c r="I13" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="57" t="s">
+    <row r="14" spans="1:9" ht="54">
+      <c r="A14" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C14" s="61" t="s">
+      <c r="C14" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="57"/>
-      <c r="F14" s="57" t="s">
+      <c r="D14" s="4"/>
+      <c r="F14" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G14" s="61" t="s">
+      <c r="G14" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="H14" s="57" t="s">
+      <c r="H14" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="I14" s="61" t="s">
+      <c r="I14" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="57" t="s">
+    <row r="15" spans="1:9" ht="54">
+      <c r="A15" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="61" t="s">
+      <c r="C15" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="57"/>
-      <c r="F15" s="57" t="s">
+      <c r="D15" s="4"/>
+      <c r="F15" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="61" t="s">
+      <c r="G15" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="H15" s="57" t="s">
+      <c r="H15" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="I15" s="61" t="s">
+      <c r="I15" s="8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="57" t="s">
+    <row r="16" spans="1:9" ht="54">
+      <c r="A16" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C16" s="61" t="s">
+      <c r="C16" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D16" s="57"/>
-      <c r="F16" s="57" t="s">
+      <c r="D16" s="4"/>
+      <c r="F16" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="G16" s="61" t="s">
+      <c r="G16" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="H16" s="57" t="s">
+      <c r="H16" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="I16" s="61" t="s">
+      <c r="I16" s="8" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="57" t="s">
+    <row r="17" spans="1:9" ht="108">
+      <c r="A17" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="61" t="s">
+      <c r="C17" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="57"/>
-      <c r="F17" s="57" t="s">
+      <c r="D17" s="4"/>
+      <c r="F17" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="G17" s="61" t="s">
+      <c r="G17" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="H17" s="57" t="s">
+      <c r="H17" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="I17" s="61" t="s">
+      <c r="I17" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="57" t="s">
+    <row r="18" spans="1:9" ht="81">
+      <c r="A18" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C18" s="61" t="s">
+      <c r="C18" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D18" s="57"/>
-      <c r="F18" s="57" t="s">
+      <c r="D18" s="4"/>
+      <c r="F18" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="G18" s="61" t="s">
+      <c r="G18" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="H18" s="57" t="s">
+      <c r="H18" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="I18" s="61" t="s">
+      <c r="I18" s="8" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="57" t="s">
+    <row r="19" spans="1:9" ht="54">
+      <c r="A19" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B19" s="57" t="s">
+      <c r="B19" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C19" s="61" t="s">
+      <c r="C19" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D19" s="57"/>
-      <c r="F19" s="57" t="s">
+      <c r="D19" s="4"/>
+      <c r="F19" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="G19" s="61" t="s">
+      <c r="G19" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="H19" s="57" t="s">
+      <c r="H19" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="I19" s="61" t="s">
+      <c r="I19" s="8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="55" t="s">
+    <row r="20" spans="1:9" ht="108">
+      <c r="A20" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C20" s="61" t="s">
+      <c r="C20" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D20" s="55"/>
-      <c r="F20" s="55" t="s">
+      <c r="D20" s="2"/>
+      <c r="F20" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="G20" s="61" t="s">
+      <c r="G20" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="H20" s="55" t="s">
+      <c r="H20" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="I20" s="61" t="s">
+      <c r="I20" s="8" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="55" t="s">
+    <row r="21" spans="1:9" ht="121.5">
+      <c r="A21" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B21" s="55" t="s">
+      <c r="B21" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C21" s="61" t="s">
+      <c r="C21" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D21" s="55"/>
-      <c r="F21" s="55" t="s">
+      <c r="D21" s="2"/>
+      <c r="F21" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="G21" s="61" t="s">
+      <c r="G21" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="H21" s="55" t="s">
+      <c r="H21" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="I21" s="61" t="s">
+      <c r="I21" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="55" t="s">
+    <row r="22" spans="1:9" ht="54">
+      <c r="A22" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B22" s="55" t="s">
+      <c r="B22" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C22" s="61" t="s">
+      <c r="C22" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D22" s="55"/>
-      <c r="F22" s="55" t="s">
+      <c r="D22" s="2"/>
+      <c r="F22" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G22" s="61" t="s">
+      <c r="G22" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="H22" s="55" t="s">
+      <c r="H22" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="I22" s="61" t="s">
+      <c r="I22" s="8" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="54" t="s">
+    <row r="23" spans="1:9" ht="94.5">
+      <c r="A23" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C23" s="61" t="s">
+      <c r="C23" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="F23" s="54" t="s">
+      <c r="F23" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="G23" s="61" t="s">
+      <c r="G23" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="H23" s="54" t="s">
+      <c r="H23" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="I23" s="61" t="s">
+      <c r="I23" s="8" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="54" t="s">
+    <row r="24" spans="1:9" ht="135">
+      <c r="A24" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B24" s="54" t="s">
+      <c r="B24" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C24" s="61" t="s">
+      <c r="C24" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="F24" s="54" t="s">
+      <c r="F24" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="G24" s="61" t="s">
+      <c r="G24" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H24" s="54" t="s">
+      <c r="H24" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="I24" s="61" t="s">
+      <c r="I24" s="8" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="54" t="s">
+    <row r="25" spans="1:9" ht="108">
+      <c r="A25" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B25" s="54" t="s">
+      <c r="B25" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C25" s="61" t="s">
+      <c r="C25" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="F25" s="54" t="s">
+      <c r="F25" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="G25" s="61" t="s">
+      <c r="G25" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="H25" s="54" t="s">
+      <c r="I25" s="8" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="108">
+      <c r="A26" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="I25" s="61" t="s">
+      <c r="B26" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="54" t="s">
+      <c r="F26" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B26" s="54" t="s">
-        <v>150</v>
-      </c>
-      <c r="C26" s="61" t="s">
+      <c r="G26" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="F26" s="54" t="s">
+      <c r="H26" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="G26" s="61" t="s">
+      <c r="I26" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="H26" s="54" t="s">
+    </row>
+    <row r="27" spans="1:9" ht="202.5">
+      <c r="A27" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I26" s="61" t="s">
+      <c r="B27" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="54" t="s">
+      <c r="D27" s="1"/>
+      <c r="F27" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B27" s="54" t="s">
-        <v>156</v>
-      </c>
-      <c r="C27" s="61" t="s">
+      <c r="G27" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="D27" s="54"/>
-      <c r="F27" s="54" t="s">
+      <c r="H27" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="G27" s="61" t="s">
+      <c r="I27" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="H27" s="54" t="s">
+    </row>
+    <row r="28" spans="1:9" ht="148.5">
+      <c r="A28" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="I27" s="61" t="s">
+      <c r="B28" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="54" t="s">
+      <c r="D28" s="1"/>
+      <c r="F28" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B28" s="54" t="s">
-        <v>162</v>
-      </c>
-      <c r="C28" s="61" t="s">
+      <c r="G28" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="D28" s="54"/>
-      <c r="F28" s="54" t="s">
+      <c r="H28" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="G28" s="61" t="s">
+      <c r="I28" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="H28" s="54" t="s">
+    </row>
+    <row r="29" spans="1:9" ht="108">
+      <c r="A29" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="I28" s="61" t="s">
+      <c r="B29" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="54" t="s">
+      <c r="D29" s="1"/>
+      <c r="F29" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B29" s="54" t="s">
-        <v>168</v>
-      </c>
-      <c r="C29" s="61" t="s">
+      <c r="G29" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="D29" s="54"/>
-      <c r="F29" s="54" t="s">
+      <c r="H29" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="G29" s="61" t="s">
+      <c r="I29" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="H29" s="54" t="s">
+    </row>
+    <row r="30" spans="1:9" ht="108">
+      <c r="A30" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I29" s="61" t="s">
+      <c r="B30" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="54" t="s">
+      <c r="D30" s="1"/>
+      <c r="F30" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B30" s="54" t="s">
-        <v>174</v>
-      </c>
-      <c r="C30" s="61" t="s">
+      <c r="G30" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="D30" s="54"/>
-      <c r="F30" s="54" t="s">
+      <c r="H30" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="G30" s="61" t="s">
+      <c r="I30" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="H30" s="54" t="s">
+    </row>
+    <row r="31" spans="1:9" ht="27">
+      <c r="A31" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="I30" s="61" t="s">
+      <c r="B31" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="54" t="s">
+      <c r="D31" s="1"/>
+      <c r="F31" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B31" s="54" t="s">
-        <v>180</v>
-      </c>
-      <c r="C31" s="61" t="s">
+      <c r="I31" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="D31" s="54"/>
-      <c r="F31" s="54" t="s">
-        <v>180</v>
-      </c>
-      <c r="G31" s="61" t="s">
-        <v>181</v>
-      </c>
-      <c r="H31" s="54" t="s">
+    </row>
+    <row r="32" spans="1:9" ht="54">
+      <c r="A32" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="I31" s="61" t="s">
+      <c r="B32" s="1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="54" t="s">
+      <c r="C32" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="B32" s="54" t="s">
+      <c r="D32" s="1"/>
+      <c r="F32" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C32" s="61" t="s">
+      <c r="G32" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="D32" s="54"/>
-      <c r="F32" s="54" t="s">
+      <c r="H32" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G32" s="61" t="s">
+      <c r="I32" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="H32" s="54" t="s">
+    </row>
+    <row r="33" spans="1:9" ht="27">
+      <c r="A33" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="I32" s="61" t="s">
+      <c r="B33" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="F33" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="54" t="s">
+      <c r="G33" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="B33" s="54" t="s">
-        <v>185</v>
-      </c>
-      <c r="C33" s="61" t="s">
-        <v>186</v>
-      </c>
-      <c r="D33" s="54"/>
-      <c r="F33" s="54" t="s">
+      <c r="H33" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="G33" s="61" t="s">
+      <c r="I33" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="H33" s="54" t="s">
+    </row>
+    <row r="34" spans="1:9" ht="94.5">
+      <c r="A34" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="I33" s="61" t="s">
+      <c r="B34" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="F34" s="1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="54" t="s">
+      <c r="G34" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="B34" s="54" t="s">
-        <v>185</v>
-      </c>
-      <c r="C34" s="61" t="s">
-        <v>186</v>
-      </c>
-      <c r="D34" s="54"/>
-      <c r="F34" s="54" t="s">
+      <c r="H34" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="G34" s="61" t="s">
+      <c r="I34" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="H34" s="54" t="s">
+    </row>
+    <row r="35" spans="1:9" ht="108">
+      <c r="A35" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="I34" s="61" t="s">
+      <c r="B35" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="F35" s="1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="54" t="s">
+      <c r="G35" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="B35" s="54" t="s">
-        <v>185</v>
-      </c>
-      <c r="C35" s="61" t="s">
-        <v>186</v>
-      </c>
-      <c r="D35" s="54"/>
-      <c r="F35" s="54" t="s">
+      <c r="H35" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="G35" s="61" t="s">
+      <c r="I35" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="H35" s="54" t="s">
+    </row>
+    <row r="36" spans="1:9" ht="67.5">
+      <c r="A36" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="I35" s="61" t="s">
+      <c r="B36" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="F36" s="1" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="54" t="s">
+      <c r="G36" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="B36" s="54" t="s">
-        <v>185</v>
-      </c>
-      <c r="C36" s="61" t="s">
-        <v>186</v>
-      </c>
-      <c r="D36" s="54"/>
-      <c r="F36" s="54" t="s">
+      <c r="H36" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="G36" s="61" t="s">
+      <c r="I36" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="H36" s="54" t="s">
+    </row>
+    <row r="37" spans="1:9" ht="67.5">
+      <c r="A37" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="I36" s="61" t="s">
+      <c r="B37" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="F37" s="1" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="54" t="s">
+      <c r="G37" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="B37" s="54" t="s">
-        <v>185</v>
-      </c>
-      <c r="C37" s="61" t="s">
-        <v>186</v>
-      </c>
-      <c r="D37" s="54"/>
-      <c r="F37" s="54" t="s">
+      <c r="H37" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="G37" s="61" t="s">
+      <c r="I37" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="H37" s="54" t="s">
+    </row>
+    <row r="38" spans="1:9" ht="94.5">
+      <c r="A38" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="I37" s="61" t="s">
+      <c r="B38" s="5" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="58" t="s">
+      <c r="C38" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="B38" s="58" t="s">
+      <c r="D38" s="5"/>
+      <c r="F38" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C38" s="61" t="s">
+      <c r="G38" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="D38" s="58"/>
-      <c r="F38" s="58" t="s">
+      <c r="H38" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="G38" s="61" t="s">
+      <c r="I38" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="H38" s="58" t="s">
+    </row>
+    <row r="39" spans="1:9" ht="81">
+      <c r="A39" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="I38" s="61" t="s">
+      <c r="B39" s="5" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="58" t="s">
+      <c r="C39" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="B39" s="58" t="s">
+      <c r="D39" s="5"/>
+      <c r="F39" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="C39" s="61" t="s">
+      <c r="G39" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="D39" s="58"/>
-      <c r="F39" s="58" t="s">
+      <c r="H39" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="G39" s="61" t="s">
+      <c r="I39" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="H39" s="58" t="s">
+    </row>
+    <row r="40" spans="1:9" ht="67.5">
+      <c r="A40" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="I39" s="61" t="s">
+      <c r="B40" s="5" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="58" t="s">
+      <c r="C40" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="B40" s="58" t="s">
+      <c r="D40" s="5"/>
+      <c r="F40" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="C40" s="61" t="s">
+      <c r="G40" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="D40" s="58"/>
-      <c r="F40" s="58" t="s">
+      <c r="H40" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="G40" s="61" t="s">
+      <c r="I40" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="H40" s="58" t="s">
+    </row>
+    <row r="41" spans="1:9" ht="108">
+      <c r="A41" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="I40" s="61" t="s">
+      <c r="B41" s="5" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="58" t="s">
+      <c r="C41" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="B41" s="58" t="s">
+      <c r="D41" s="5"/>
+      <c r="F41" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="C41" s="61" t="s">
+      <c r="G41" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="D41" s="58"/>
-      <c r="F41" s="58" t="s">
+      <c r="H41" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="G41" s="61" t="s">
+      <c r="I41" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="H41" s="58" t="s">
+    </row>
+    <row r="42" spans="1:9" ht="94.5">
+      <c r="A42" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="I41" s="61" t="s">
+      <c r="B42" s="5" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="58" t="s">
+      <c r="C42" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="B42" s="58" t="s">
+      <c r="D42" s="5"/>
+      <c r="F42" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="C42" s="61" t="s">
+      <c r="G42" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="D42" s="58"/>
-      <c r="F42" s="58" t="s">
+      <c r="H42" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="G42" s="61" t="s">
+      <c r="I42" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="H42" s="58" t="s">
-        <v>249</v>
-      </c>
-      <c r="I42" s="61" t="s">
-        <v>250</v>
-      </c>
     </row>
   </sheetData>
-  <headerFooter/>
-  <legacyDrawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>